<commit_message>
Fixed headers in test data
</commit_message>
<xml_diff>
--- a/excelData/blenderFactory.xlsx
+++ b/excelData/blenderFactory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/excelData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{542083C6-EFDF-4E45-A343-C4DCE5F0D845}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFBA0A70-CFFD-634A-925A-20DE382E3F08}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="460" windowWidth="27640" windowHeight="16540" activeTab="2" xr2:uid="{EAC7D76D-1E0E-F74E-87ED-1328504900CF}"/>
+    <workbookView xWindow="1160" yWindow="460" windowWidth="27640" windowHeight="16540" activeTab="1" xr2:uid="{EAC7D76D-1E0E-F74E-87ED-1328504900CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Chain List" sheetId="1" r:id="rId1"/>
@@ -108,12 +108,6 @@
     <t>ChainSheet</t>
   </si>
   <si>
-    <t>OriginChain</t>
-  </si>
-  <si>
-    <t>OriginProcess</t>
-  </si>
-  <si>
     <t>Product</t>
   </si>
   <si>
@@ -123,9 +117,6 @@
     <t>Product_IO_of_Destination</t>
   </si>
   <si>
-    <t>DestinationChain</t>
-  </si>
-  <si>
     <t>all</t>
   </si>
   <si>
@@ -154,6 +145,15 @@
   </si>
   <si>
     <t>Blender Chain</t>
+  </si>
+  <si>
+    <t>Origin_Chain</t>
+  </si>
+  <si>
+    <t>Origin_Unit</t>
+  </si>
+  <si>
+    <t>Destination_Chain</t>
   </si>
 </sst>
 </file>
@@ -551,7 +551,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -560,7 +560,7 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -574,7 +574,7 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -586,8 +586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52AFC89D-04CC-084A-B745-788782739698}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -602,30 +602,30 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" t="s">
-        <v>13</v>
-      </c>
       <c r="F1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -649,7 +649,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72EF0295-B8C2-BB45-9AF7-94BDD97678E5}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -662,21 +662,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -704,21 +704,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>

</xml_diff>